<commit_message>
[2.0.0] Cập nhật lớn
- Sửa đổi toàn bộ cấu trúc thư mục
- Cập nhật hệ thống log cho trận đấu
- Cập nhật hệ thống đọc tên thí sinh và điểm từ file excel
- Cập nhật tính năng chọn mở/đóng khoá chuông 3s sau khi qua câu hỏi mới ở Khởi động
- Cập nhật âm thanh cho Khởi động
- Sửa đổi UI hiện đáp án hàng ngang Chướng ngại vật và Tăng tốc
- Cập nhật vị trí tín hiệu Chướng ngại vật ở các UI đáp án thí sinh và ảnh
- Cập nhật điều chỉnh âm lượng ở máy thí sinh
- Cập nhật hệ thống đặt lại trạng thái vòng thi ở Vượt chướng ngại vật
- Sửa font chữ tên vòng thi ở viewer và tên thí sinh ở trang điểm số
- Fix hàng loạt các bug và điều chỉnh logic hoạt động của code
</commit_message>
<xml_diff>
--- a/Form nhập đề.xlsx
+++ b/Form nhập đề.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2. O Project\Olympia_24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2. O Project\Olympia_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207D4774-8D89-49CD-9673-51D6432E3C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D84F10E-D387-44B2-8804-19F1DA89FF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1E2E1B2-ECC6-431A-9DB1-D10D877A3DFD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{D1E2E1B2-ECC6-431A-9DB1-D10D877A3DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction" sheetId="7" r:id="rId1"/>
@@ -158,15 +158,44 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t>Một hàng ngang chỉ hỗ trợ hiển thị ở viewer tối đa 18 kí tự, vị trí bắt đầu từ 1-&gt;18. Sau đây là bảng chọn vị trí của kí tự đầu tiên trong mỗi hàng. Nếu bạn không cần tuỳ chỉnh, vui lòng điền vào ô vị trí bắt đầu theo giá trị được khuyến nghị</t>
+      <t>Một hàng ngang chỉ hỗ trợ hiển thị ở viewer tối đa 18 kí tự, vị trí bắt đầu từ 1-&gt;18. Sau đây là bảng chọn vị trí của kí tự đầu tiên trong mỗi hàng. Nếu bạn không cần tuỳ chỉnh, vui lòng điền vào ô vị trí bắt đầu theo giá trị được khuyến nghị.</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1. File video nên là file .mp4
-2. File âm thanh nên là file .mp3 hoặc .wav
-3. File hình ảnh nên là file .jpg hoặc .png
-4. Các file media ở mục 1, 2, 3 có thể ở bất kì đâu bắt đầu từ folder </t>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> Định dạng file video nên là mp4, với hình ảnh là jpg, jpeg hoặc png, với audio là mp3 hoặc wav.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> Các file media ở mục 1 có thể ở bất kì đâu bắt đầu từ folder </t>
     </r>
     <r>
       <rPr>
@@ -185,45 +214,7 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve"> trở đi. Cú pháp cho đầu đường dẫn có thể là không có gì, hoặc là "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-        <charset val="163"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-        <charset val="163"/>
-      </rPr>
-      <t>", hoặc là "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-        <charset val="163"/>
-      </rPr>
-      <t>./</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">". Bạn có thể tự tạo thêm folder trong public (Ví dụ, file ảnh chướng ngại vật của bạn là </t>
+      <t xml:space="preserve"> trở đi. Bạn có thể tự tạo thêm folder trong public (Ví dụ, file ảnh chướng ngại vật của bạn là </t>
     </r>
     <r>
       <rPr>
@@ -299,7 +290,7 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve">, thì đường dẫn của bạn có thể là </t>
+      <t>, thì đường dẫn của bạn là</t>
     </r>
     <r>
       <rPr>
@@ -307,9 +298,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Montserrat"/>
-        <charset val="163"/>
       </rPr>
-      <t>image/obs.png</t>
+      <t xml:space="preserve"> /public/image/obs.png</t>
     </r>
     <r>
       <rPr>
@@ -318,7 +308,8 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t xml:space="preserve">).
+</t>
     </r>
     <r>
       <rPr>
@@ -326,9 +317,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Montserrat"/>
-        <charset val="163"/>
       </rPr>
-      <t>/image/obs.png</t>
+      <t>3.</t>
     </r>
     <r>
       <rPr>
@@ -337,27 +327,7 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve"> ./image/obs.png</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-        <charset val="163"/>
-      </rPr>
-      <t xml:space="preserve">)
-5. Để kiểm tra các media đã được load thành công vào server hay chưa, truy cập vào </t>
+      <t xml:space="preserve"> Để kiểm tra các media đã được load thành công vào server hay chưa, truy cập vào </t>
     </r>
     <r>
       <rPr>
@@ -376,7 +346,7 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve"> (Ví dụ với file ảnh ở trên mục 4, địa chỉ kiểm tra media với IP </t>
+      <t xml:space="preserve"> (Ví dụ với file ảnh ở trên mục 2, địa chỉ kiểm tra media với IP </t>
     </r>
     <r>
       <rPr>
@@ -424,7 +394,15 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve">192.168.0.100:3000/image/obs.png </t>
+      <t>192.168.0.100:3000/public/image/obs.png</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>).</t>
     </r>
     <r>
       <rPr>
@@ -433,7 +411,8 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve">(không có dấu chấm </t>
+      <t xml:space="preserve">
+</t>
     </r>
     <r>
       <rPr>
@@ -441,9 +420,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Montserrat"/>
-        <charset val="163"/>
       </rPr>
-      <t>.</t>
+      <t>6.</t>
     </r>
     <r>
       <rPr>
@@ -452,7 +430,8 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t xml:space="preserve"> trước dấu gạch </t>
+      <t xml:space="preserve"> Khi nhập đề, chỉ được nhập vào những ô không được tô màu (màu trắng).
+</t>
     </r>
     <r>
       <rPr>
@@ -460,9 +439,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Montserrat"/>
-        <charset val="163"/>
       </rPr>
-      <t>/</t>
+      <t>7.</t>
     </r>
     <r>
       <rPr>
@@ -471,10 +449,26 @@
         <rFont val="Montserrat"/>
         <charset val="163"/>
       </rPr>
-      <t>)
-5. Khi nhập đề, chỉ được nhập vào những ô không được tô màu (màu trắng)
-6. Không được đổi tên các sheet phần thi được tô màu
-7. Đối với các đáp án phục vụ cho việc đếm số kí tự như hàng ngang và chướng ngại vật, chỉ được ghi 1 đáp án đúng duy nhất, không được chú thích thêm. Nên nhập đáp án đầy đủ dấu và khoảng trắng</t>
+      <t xml:space="preserve"> Không được đổi tên các sheet phần thi được tô màu.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+        <charset val="163"/>
+      </rPr>
+      <t>. Đối với các đáp án phục vụ cho việc đếm số kí tự như hàng ngang và Chướng ngại vật, chỉ được ghi 1 đáp án đúng duy nhất. Nên nhập đáp án đầy đủ dấu và khoảng trắng.</t>
     </r>
   </si>
 </sst>
@@ -482,11 +476,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -510,6 +504,17 @@
       <color theme="1"/>
       <name val="Montserrat"/>
       <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
     </font>
   </fonts>
   <fills count="8">
@@ -556,7 +561,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="77">
+  <borders count="70">
     <border>
       <left/>
       <right/>
@@ -1465,83 +1470,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1596,7 +1530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1944,6 +1878,27 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1980,53 +1935,17 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2356,71 +2275,71 @@
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+    <row r="1" spans="1:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="134"/>
-      <c r="E1" s="132" t="s">
+      <c r="B1" s="121"/>
+      <c r="C1" s="122"/>
+      <c r="E1" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="134"/>
-    </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="131" t="s">
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="122"/>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="131" t="s">
+      <c r="B2" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="131" t="s">
+      <c r="C2" s="119" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="138" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="136"/>
-      <c r="M2" s="139"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="129">
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="117">
         <v>1</v>
       </c>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="140"/>
+      <c r="E3" s="137"/>
       <c r="F3" s="137"/>
       <c r="G3" s="137"/>
       <c r="H3" s="137"/>
@@ -2428,19 +2347,19 @@
       <c r="J3" s="137"/>
       <c r="K3" s="137"/>
       <c r="L3" s="137"/>
-      <c r="M3" s="141"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="129">
+      <c r="M3" s="137"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="117">
         <v>2</v>
       </c>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="129" t="s">
+      <c r="C4" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="140"/>
+      <c r="E4" s="137"/>
       <c r="F4" s="137"/>
       <c r="G4" s="137"/>
       <c r="H4" s="137"/>
@@ -2448,19 +2367,19 @@
       <c r="J4" s="137"/>
       <c r="K4" s="137"/>
       <c r="L4" s="137"/>
-      <c r="M4" s="141"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="129">
+      <c r="M4" s="137"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="117">
         <v>3</v>
       </c>
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="129" t="s">
+      <c r="C5" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="140"/>
+      <c r="E5" s="137"/>
       <c r="F5" s="137"/>
       <c r="G5" s="137"/>
       <c r="H5" s="137"/>
@@ -2468,19 +2387,19 @@
       <c r="J5" s="137"/>
       <c r="K5" s="137"/>
       <c r="L5" s="137"/>
-      <c r="M5" s="141"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="129">
+      <c r="M5" s="137"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="117">
         <v>4</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="129" t="s">
+      <c r="C6" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="140"/>
+      <c r="E6" s="137"/>
       <c r="F6" s="137"/>
       <c r="G6" s="137"/>
       <c r="H6" s="137"/>
@@ -2488,19 +2407,19 @@
       <c r="J6" s="137"/>
       <c r="K6" s="137"/>
       <c r="L6" s="137"/>
-      <c r="M6" s="141"/>
-    </row>
-    <row r="7" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="130">
+      <c r="M6" s="137"/>
+    </row>
+    <row r="7" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="118">
         <v>5</v>
       </c>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="140"/>
+      <c r="E7" s="137"/>
       <c r="F7" s="137"/>
       <c r="G7" s="137"/>
       <c r="H7" s="137"/>
@@ -2508,10 +2427,10 @@
       <c r="J7" s="137"/>
       <c r="K7" s="137"/>
       <c r="L7" s="137"/>
-      <c r="M7" s="141"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E8" s="140"/>
+      <c r="M7" s="137"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E8" s="137"/>
       <c r="F8" s="137"/>
       <c r="G8" s="137"/>
       <c r="H8" s="137"/>
@@ -2519,10 +2438,10 @@
       <c r="J8" s="137"/>
       <c r="K8" s="137"/>
       <c r="L8" s="137"/>
-      <c r="M8" s="141"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E9" s="140"/>
+      <c r="M8" s="137"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E9" s="137"/>
       <c r="F9" s="137"/>
       <c r="G9" s="137"/>
       <c r="H9" s="137"/>
@@ -2530,10 +2449,10 @@
       <c r="J9" s="137"/>
       <c r="K9" s="137"/>
       <c r="L9" s="137"/>
-      <c r="M9" s="141"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E10" s="140"/>
+      <c r="M9" s="137"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E10" s="137"/>
       <c r="F10" s="137"/>
       <c r="G10" s="137"/>
       <c r="H10" s="137"/>
@@ -2541,10 +2460,10 @@
       <c r="J10" s="137"/>
       <c r="K10" s="137"/>
       <c r="L10" s="137"/>
-      <c r="M10" s="141"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E11" s="140"/>
+      <c r="M10" s="137"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E11" s="137"/>
       <c r="F11" s="137"/>
       <c r="G11" s="137"/>
       <c r="H11" s="137"/>
@@ -2552,10 +2471,10 @@
       <c r="J11" s="137"/>
       <c r="K11" s="137"/>
       <c r="L11" s="137"/>
-      <c r="M11" s="141"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E12" s="140"/>
+      <c r="M11" s="137"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="137"/>
       <c r="F12" s="137"/>
       <c r="G12" s="137"/>
       <c r="H12" s="137"/>
@@ -2563,10 +2482,10 @@
       <c r="J12" s="137"/>
       <c r="K12" s="137"/>
       <c r="L12" s="137"/>
-      <c r="M12" s="141"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E13" s="140"/>
+      <c r="M12" s="137"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E13" s="137"/>
       <c r="F13" s="137"/>
       <c r="G13" s="137"/>
       <c r="H13" s="137"/>
@@ -2574,10 +2493,10 @@
       <c r="J13" s="137"/>
       <c r="K13" s="137"/>
       <c r="L13" s="137"/>
-      <c r="M13" s="141"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E14" s="140"/>
+      <c r="M13" s="137"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E14" s="137"/>
       <c r="F14" s="137"/>
       <c r="G14" s="137"/>
       <c r="H14" s="137"/>
@@ -2585,10 +2504,10 @@
       <c r="J14" s="137"/>
       <c r="K14" s="137"/>
       <c r="L14" s="137"/>
-      <c r="M14" s="141"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E15" s="140"/>
+      <c r="M14" s="137"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E15" s="137"/>
       <c r="F15" s="137"/>
       <c r="G15" s="137"/>
       <c r="H15" s="137"/>
@@ -2596,10 +2515,10 @@
       <c r="J15" s="137"/>
       <c r="K15" s="137"/>
       <c r="L15" s="137"/>
-      <c r="M15" s="141"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E16" s="140"/>
+      <c r="M15" s="137"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E16" s="137"/>
       <c r="F16" s="137"/>
       <c r="G16" s="137"/>
       <c r="H16" s="137"/>
@@ -2607,10 +2526,10 @@
       <c r="J16" s="137"/>
       <c r="K16" s="137"/>
       <c r="L16" s="137"/>
-      <c r="M16" s="141"/>
-    </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
-      <c r="E17" s="140"/>
+      <c r="M16" s="137"/>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E17" s="137"/>
       <c r="F17" s="137"/>
       <c r="G17" s="137"/>
       <c r="H17" s="137"/>
@@ -2618,24 +2537,68 @@
       <c r="J17" s="137"/>
       <c r="K17" s="137"/>
       <c r="L17" s="137"/>
-      <c r="M17" s="141"/>
-    </row>
-    <row r="18" spans="5:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E18" s="142"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
-      <c r="K18" s="143"/>
-      <c r="L18" s="143"/>
-      <c r="M18" s="144"/>
+      <c r="M17" s="137"/>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="137"/>
+      <c r="F18" s="137"/>
+      <c r="G18" s="137"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="137"/>
+      <c r="J18" s="137"/>
+      <c r="K18" s="137"/>
+      <c r="L18" s="137"/>
+      <c r="M18" s="137"/>
+    </row>
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="137"/>
+      <c r="F19" s="137"/>
+      <c r="G19" s="137"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="137"/>
+      <c r="J19" s="137"/>
+      <c r="K19" s="137"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="137"/>
+    </row>
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E20" s="137"/>
+      <c r="F20" s="137"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="137"/>
+      <c r="K20" s="137"/>
+      <c r="L20" s="137"/>
+      <c r="M20" s="137"/>
+    </row>
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E21" s="137"/>
+      <c r="F21" s="137"/>
+      <c r="G21" s="137"/>
+      <c r="H21" s="137"/>
+      <c r="I21" s="137"/>
+      <c r="J21" s="137"/>
+      <c r="K21" s="137"/>
+      <c r="L21" s="137"/>
+      <c r="M21" s="137"/>
+    </row>
+    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E22" s="137"/>
+      <c r="F22" s="137"/>
+      <c r="G22" s="137"/>
+      <c r="H22" s="137"/>
+      <c r="I22" s="137"/>
+      <c r="J22" s="137"/>
+      <c r="K22" s="137"/>
+      <c r="L22" s="137"/>
+      <c r="M22" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:M1"/>
-    <mergeCell ref="E2:M18"/>
+    <mergeCell ref="E2:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2652,18 +2615,18 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="18.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="36" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.75" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.75" style="71" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="71" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2686,8 +2649,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="117">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="124">
         <v>1</v>
       </c>
       <c r="B2" s="109">
@@ -2701,8 +2664,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="118"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="125"/>
       <c r="B3" s="110">
         <v>2</v>
       </c>
@@ -2714,8 +2677,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="118"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="125"/>
       <c r="B4" s="110">
         <v>3</v>
       </c>
@@ -2727,8 +2690,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="118"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="125"/>
       <c r="B5" s="110">
         <v>4</v>
       </c>
@@ -2740,8 +2703,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="118"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="125"/>
       <c r="B6" s="110">
         <v>5</v>
       </c>
@@ -2753,8 +2716,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="118"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="125"/>
       <c r="B7" s="110">
         <v>6</v>
       </c>
@@ -2766,8 +2729,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="119">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="126">
         <v>2</v>
       </c>
       <c r="B8" s="111">
@@ -2781,8 +2744,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="119"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="126"/>
       <c r="B9" s="110">
         <v>2</v>
       </c>
@@ -2794,8 +2757,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="119"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="126"/>
       <c r="B10" s="110">
         <v>3</v>
       </c>
@@ -2807,8 +2770,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="119"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="126"/>
       <c r="B11" s="110">
         <v>4</v>
       </c>
@@ -2820,8 +2783,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="119"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="126"/>
       <c r="B12" s="110">
         <v>5</v>
       </c>
@@ -2833,8 +2796,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="119"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="126"/>
       <c r="B13" s="110">
         <v>6</v>
       </c>
@@ -2846,8 +2809,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="119">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="126">
         <v>3</v>
       </c>
       <c r="B14" s="111">
@@ -2861,8 +2824,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="119"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="126"/>
       <c r="B15" s="110">
         <v>2</v>
       </c>
@@ -2874,8 +2837,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="119"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="126"/>
       <c r="B16" s="110">
         <v>3</v>
       </c>
@@ -2887,8 +2850,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="119"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="126"/>
       <c r="B17" s="110">
         <v>4</v>
       </c>
@@ -2900,8 +2863,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="119"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="126"/>
       <c r="B18" s="110">
         <v>5</v>
       </c>
@@ -2913,8 +2876,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="119"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="126"/>
       <c r="B19" s="110">
         <v>6</v>
       </c>
@@ -2926,8 +2889,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="119">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="126">
         <v>4</v>
       </c>
       <c r="B20" s="111">
@@ -2941,8 +2904,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="119"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="126"/>
       <c r="B21" s="110">
         <v>2</v>
       </c>
@@ -2954,8 +2917,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="119"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="126"/>
       <c r="B22" s="110">
         <v>3</v>
       </c>
@@ -2967,8 +2930,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="119"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="126"/>
       <c r="B23" s="110">
         <v>4</v>
       </c>
@@ -2980,8 +2943,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="119"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="126"/>
       <c r="B24" s="110">
         <v>5</v>
       </c>
@@ -2993,8 +2956,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="120"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="127"/>
       <c r="B25" s="112">
         <v>6</v>
       </c>
@@ -3006,8 +2969,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="121">
+    <row r="26" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="128">
         <v>5</v>
       </c>
       <c r="B26" s="113">
@@ -3021,8 +2984,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="122"/>
+    <row r="27" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="129"/>
       <c r="B27" s="114">
         <v>2</v>
       </c>
@@ -3034,8 +2997,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="122"/>
+    <row r="28" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="129"/>
       <c r="B28" s="114">
         <v>3</v>
       </c>
@@ -3047,8 +3010,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="122"/>
+    <row r="29" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="129"/>
       <c r="B29" s="114">
         <v>4</v>
       </c>
@@ -3060,8 +3023,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="122"/>
+    <row r="30" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="129"/>
       <c r="B30" s="114">
         <v>5</v>
       </c>
@@ -3073,8 +3036,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="122"/>
+    <row r="31" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="129"/>
       <c r="B31" s="114">
         <v>6</v>
       </c>
@@ -3086,8 +3049,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="122"/>
+    <row r="32" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="129"/>
       <c r="B32" s="115">
         <v>7</v>
       </c>
@@ -3099,8 +3062,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="122"/>
+    <row r="33" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="129"/>
       <c r="B33" s="115">
         <v>8</v>
       </c>
@@ -3112,8 +3075,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="122"/>
+    <row r="34" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="129"/>
       <c r="B34" s="115">
         <v>9</v>
       </c>
@@ -3125,8 +3088,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="122"/>
+    <row r="35" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="129"/>
       <c r="B35" s="115">
         <v>10</v>
       </c>
@@ -3138,8 +3101,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="122"/>
+    <row r="36" spans="1:7" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="129"/>
       <c r="B36" s="115">
         <v>11</v>
       </c>
@@ -3151,8 +3114,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="71" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="123"/>
+    <row r="37" spans="1:7" s="71" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="130"/>
       <c r="B37" s="116">
         <v>12</v>
       </c>
@@ -3185,19 +3148,19 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="55.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.75" style="2" customWidth="1"/>
-    <col min="5" max="6" width="39.25" style="2" customWidth="1"/>
+    <col min="1" max="2" width="18.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="39.28515625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>7</v>
       </c>
@@ -3217,7 +3180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="47">
         <v>1</v>
       </c>
@@ -3230,7 +3193,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="49">
         <v>2</v>
       </c>
@@ -3243,7 +3206,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="49">
         <v>3</v>
       </c>
@@ -3256,7 +3219,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="49">
         <v>4</v>
       </c>
@@ -3269,7 +3232,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="49">
         <v>5</v>
       </c>
@@ -3282,7 +3245,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
         <v>8</v>
       </c>
@@ -3295,15 +3258,17 @@
       <c r="E7" s="11"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="9" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="135" t="s">
+    <row r="9" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="135"/>
-      <c r="D9" s="135"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="136"/>
+      <c r="C9" s="136"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
         <v>12</v>
       </c>
@@ -3317,7 +3282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="91">
         <v>1</v>
       </c>
@@ -3331,7 +3296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="95">
         <v>2</v>
       </c>
@@ -3345,7 +3310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="95">
         <v>3</v>
       </c>
@@ -3359,7 +3324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="99">
         <v>4</v>
       </c>
@@ -3375,7 +3340,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3390,15 +3355,15 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
     <col min="2" max="2" width="34" style="3" customWidth="1"/>
-    <col min="3" max="4" width="35.125" style="3" customWidth="1"/>
-    <col min="5" max="7" width="35.25" style="3" customWidth="1"/>
+    <col min="3" max="4" width="35.140625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="35.28515625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -3475,6 +3440,11 @@
       <c r="H5" s="71"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{30E610C0-6931-4EDE-B418-F6721723C831}">
+      <formula1>"Image,Video"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3491,16 +3461,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="87" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="33" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>6</v>
       </c>
@@ -3520,8 +3490,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="124">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="131">
         <v>1</v>
       </c>
       <c r="B2" s="63">
@@ -3532,8 +3502,8 @@
       <c r="E2" s="19"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="124"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="131"/>
       <c r="B3" s="61">
         <v>20</v>
       </c>
@@ -3542,8 +3512,8 @@
       <c r="E3" s="19"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="124"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="131"/>
       <c r="B4" s="62">
         <v>20</v>
       </c>
@@ -3552,8 +3522,8 @@
       <c r="E4" s="19"/>
       <c r="F4" s="32"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="124"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="131"/>
       <c r="B5" s="63">
         <v>30</v>
       </c>
@@ -3562,8 +3532,8 @@
       <c r="E5" s="19"/>
       <c r="F5" s="32"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="124"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="131"/>
       <c r="B6" s="61">
         <v>30</v>
       </c>
@@ -3572,8 +3542,8 @@
       <c r="E6" s="19"/>
       <c r="F6" s="32"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="125"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="132"/>
       <c r="B7" s="64">
         <v>30</v>
       </c>
@@ -3582,8 +3552,8 @@
       <c r="E7" s="35"/>
       <c r="F7" s="33"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="126">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="133">
         <v>2</v>
       </c>
       <c r="B8" s="61">
@@ -3594,8 +3564,8 @@
       <c r="E8" s="19"/>
       <c r="F8" s="32"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="126"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
       <c r="B9" s="61">
         <v>20</v>
       </c>
@@ -3604,8 +3574,8 @@
       <c r="E9" s="19"/>
       <c r="F9" s="32"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="126"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="133"/>
       <c r="B10" s="61">
         <v>20</v>
       </c>
@@ -3614,8 +3584,8 @@
       <c r="E10" s="19"/>
       <c r="F10" s="32"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="126"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="133"/>
       <c r="B11" s="61">
         <v>30</v>
       </c>
@@ -3624,8 +3594,8 @@
       <c r="E11" s="19"/>
       <c r="F11" s="32"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="126"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="133"/>
       <c r="B12" s="61">
         <v>30</v>
       </c>
@@ -3634,8 +3604,8 @@
       <c r="E12" s="19"/>
       <c r="F12" s="32"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="127"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="134"/>
       <c r="B13" s="64">
         <v>30</v>
       </c>
@@ -3644,8 +3614,8 @@
       <c r="E13" s="35"/>
       <c r="F13" s="33"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="126">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="133">
         <v>3</v>
       </c>
       <c r="B14" s="61">
@@ -3656,8 +3626,8 @@
       <c r="E14" s="19"/>
       <c r="F14" s="32"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="126"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="133"/>
       <c r="B15" s="61">
         <v>20</v>
       </c>
@@ -3666,8 +3636,8 @@
       <c r="E15" s="19"/>
       <c r="F15" s="32"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="126"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="133"/>
       <c r="B16" s="61">
         <v>20</v>
       </c>
@@ -3676,8 +3646,8 @@
       <c r="E16" s="19"/>
       <c r="F16" s="32"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="126"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="133"/>
       <c r="B17" s="61">
         <v>30</v>
       </c>
@@ -3686,8 +3656,8 @@
       <c r="E17" s="19"/>
       <c r="F17" s="32"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="126"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="133"/>
       <c r="B18" s="61">
         <v>30</v>
       </c>
@@ -3696,8 +3666,8 @@
       <c r="E18" s="19"/>
       <c r="F18" s="32"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="127"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="134"/>
       <c r="B19" s="64">
         <v>30</v>
       </c>
@@ -3706,8 +3676,8 @@
       <c r="E19" s="35"/>
       <c r="F19" s="33"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="126">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="133">
         <v>4</v>
       </c>
       <c r="B20" s="61">
@@ -3718,8 +3688,8 @@
       <c r="E20" s="19"/>
       <c r="F20" s="32"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="126"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="133"/>
       <c r="B21" s="61">
         <v>20</v>
       </c>
@@ -3728,8 +3698,8 @@
       <c r="E21" s="19"/>
       <c r="F21" s="32"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="126"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="133"/>
       <c r="B22" s="61">
         <v>20</v>
       </c>
@@ -3738,8 +3708,8 @@
       <c r="E22" s="19"/>
       <c r="F22" s="32"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="126"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="133"/>
       <c r="B23" s="61">
         <v>30</v>
       </c>
@@ -3748,8 +3718,8 @@
       <c r="E23" s="19"/>
       <c r="F23" s="32"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="126"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="133"/>
       <c r="B24" s="61">
         <v>30</v>
       </c>
@@ -3758,8 +3728,8 @@
       <c r="E24" s="19"/>
       <c r="F24" s="32"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="128"/>
+    <row r="25" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="135"/>
       <c r="B25" s="65">
         <v>30</v>
       </c>
@@ -3786,20 +3756,20 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="73" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="34.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="34.42578125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
@@ -3816,7 +3786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="58">
         <v>1</v>
       </c>
@@ -3825,7 +3795,7 @@
       <c r="D2" s="13"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -3834,7 +3804,7 @@
       <c r="D3" s="14"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="60">
         <v>3</v>
       </c>

</xml_diff>